<commit_message>
-- document generator added +  barchart added
</commit_message>
<xml_diff>
--- a/TrainingSystem/Examples/Evaluations/GettingStarted/input/Evaluations_24_10_2023.xlsx
+++ b/TrainingSystem/Examples/Evaluations/GettingStarted/input/Evaluations_24_10_2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bvanacker/Documents/00_Development/03_RemoteRepositories/WalhoeveProjects/TrainingSystem/Examples/Evaluations/GettingStarted/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AC591C5-87E2-F741-96EA-23E637DCA5E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{973ED7DE-94ED-DA4F-92AA-DBABEF14BDA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{7E63B6CF-37E1-6B4D-8134-006C68AA0125}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$P$1:$P$49</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$P$49</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="126">
   <si>
     <t>Submission Date</t>
   </si>
@@ -380,13 +380,7 @@
     <t>was eerder kort</t>
   </si>
   <si>
-    <t>workshop ergonomie door Liantis</t>
-  </si>
-  <si>
     <t>sprak snel, wilde heel veel aanbrengen in een uur.</t>
-  </si>
-  <si>
-    <t>verzorging van baby's en jonge kinderen door Expertisecentrum kraamzorg De Wieg</t>
   </si>
   <si>
     <t>Niet echt veel van bijgeleerd, wel goed ter verfrissing</t>
@@ -799,11 +793,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89B62121-9C35-9941-B06C-95D850CA107C}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:P49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="P56" sqref="P56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J54" sqref="J54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -863,7 +856,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>44978.432719907411</v>
       </c>
@@ -898,10 +891,10 @@
       </c>
       <c r="O2" s="3"/>
       <c r="P2" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>44994.65697916667</v>
       </c>
@@ -936,10 +929,10 @@
       </c>
       <c r="O3" s="3"/>
       <c r="P3" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>45055.461863425924</v>
       </c>
@@ -974,10 +967,10 @@
       </c>
       <c r="O4" s="3"/>
       <c r="P4" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>45055.636087962965</v>
       </c>
@@ -1012,10 +1005,10 @@
       </c>
       <c r="O5" s="3"/>
       <c r="P5" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>45055.643287037034</v>
       </c>
@@ -1058,10 +1051,10 @@
         <v>27</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>45061.587361111109</v>
       </c>
@@ -1096,7 +1089,7 @@
       </c>
       <c r="O7" s="3"/>
       <c r="P7" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
@@ -1405,7 +1398,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>45085.569594907407</v>
       </c>
@@ -1471,7 +1464,9 @@
         <v>3</v>
       </c>
       <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
+      <c r="L16" s="3">
+        <v>4</v>
+      </c>
       <c r="M16" s="3"/>
       <c r="N16" s="3">
         <v>5</v>
@@ -1481,7 +1476,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>45085.61614583333</v>
       </c>
@@ -1523,7 +1518,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>45085.631504629629</v>
       </c>
@@ -1605,7 +1600,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>45100.402442129627</v>
       </c>
@@ -1643,7 +1638,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>45117.428425925929</v>
       </c>
@@ -1683,7 +1678,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="22" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>45117.445057870369</v>
       </c>
@@ -1721,7 +1716,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="23" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>45195.622812499998</v>
       </c>
@@ -1763,7 +1758,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="24" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>45208.739988425928</v>
       </c>
@@ -1803,7 +1798,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="25" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>45208.742847222224</v>
       </c>
@@ -1849,7 +1844,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="26" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>45209.405358796299</v>
       </c>
@@ -1889,7 +1884,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="27" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>45209.406122685185</v>
       </c>
@@ -1929,7 +1924,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="28" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>45209.411249999997</v>
       </c>
@@ -1967,7 +1962,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="29" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>45209.412488425929</v>
       </c>
@@ -2005,7 +2000,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="30" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>45209.417557870373</v>
       </c>
@@ -2045,7 +2040,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="31" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>45209.419861111113</v>
       </c>
@@ -2085,7 +2080,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="32" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>45209.552245370367</v>
       </c>
@@ -2123,7 +2118,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>45209.587152777778</v>
       </c>
@@ -2161,7 +2156,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="34" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>45209.592465277776</v>
       </c>
@@ -2199,7 +2194,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="35" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>45209.598032407404</v>
       </c>
@@ -2237,7 +2232,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="36" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>45209.601157407407</v>
       </c>
@@ -2279,7 +2274,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="37" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>45209.606249999997</v>
       </c>
@@ -2323,7 +2318,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="38" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>45209.953159722223</v>
       </c>
@@ -2363,7 +2358,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="39" spans="1:16" ht="239" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:16" ht="239" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>45209.955312500002</v>
       </c>
@@ -2407,7 +2402,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="40" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>45210.429340277777</v>
       </c>
@@ -2449,7 +2444,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="41" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>45210.61824074074</v>
       </c>
@@ -2487,7 +2482,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="42" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>45210.637106481481</v>
       </c>
@@ -2524,10 +2519,10 @@
       </c>
       <c r="O42" s="3"/>
       <c r="P42" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>45210.639178240737</v>
       </c>
@@ -2545,7 +2540,7 @@
         <v>4</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H43" s="3">
         <v>4</v>
@@ -2564,10 +2559,10 @@
       </c>
       <c r="O43" s="3"/>
       <c r="P43" s="3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>45210.645011574074</v>
       </c>
@@ -2581,7 +2576,7 @@
         <v>4</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F44" s="3">
         <v>4</v>
@@ -2597,13 +2592,13 @@
         <v>3</v>
       </c>
       <c r="K44" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="L44" s="3">
         <v>3</v>
       </c>
       <c r="M44" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="N44" s="3">
         <v>3</v>
@@ -2615,7 +2610,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="45" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>45211.47552083333</v>
       </c>
@@ -2637,7 +2632,9 @@
         <v>5</v>
       </c>
       <c r="I45" s="3"/>
-      <c r="J45" s="3"/>
+      <c r="J45" s="3">
+        <v>4</v>
+      </c>
       <c r="K45" s="3"/>
       <c r="L45" s="3">
         <v>3</v>
@@ -2651,7 +2648,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="46" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>45211.476689814815</v>
       </c>
@@ -2689,7 +2686,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="47" spans="1:16" ht="239" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:16" ht="239" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>45217.64980324074</v>
       </c>
@@ -2723,13 +2720,13 @@
         <v>4</v>
       </c>
       <c r="O47" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="P47" s="3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16" hidden="1" x14ac:dyDescent="0.2">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>45223.594930555555</v>
       </c>
@@ -2743,7 +2740,7 @@
         <v>4</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F48" s="3">
         <v>5</v>
@@ -2761,7 +2758,7 @@
         <v>3</v>
       </c>
       <c r="M48" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="N48" s="3">
         <v>4</v>
@@ -2771,7 +2768,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="49" spans="1:16" ht="239" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:16" ht="239" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>45223.599502314813</v>
       </c>
@@ -2785,13 +2782,13 @@
         <v>3</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F49" s="3">
         <v>3</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H49" s="3">
         <v>5</v>
@@ -2801,13 +2798,13 @@
         <v>3</v>
       </c>
       <c r="K49" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="L49" s="3">
         <v>4</v>
       </c>
       <c r="M49" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="N49" s="3">
         <v>3</v>
@@ -2818,14 +2815,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="P1:P49" xr:uid="{89B62121-9C35-9941-B06C-95D850CA107C}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="intervisie Cross Link ivm AD (verblijf) op vraag"/>
-        <filter val="intervisie Cross Link ivm AD (verblijf) op vraag."/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:P49" xr:uid="{89B62121-9C35-9941-B06C-95D850CA107C}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>